<commit_message>
first commit from after all fixes
</commit_message>
<xml_diff>
--- a/public_html/excel_demo/packet-booking-demo.xlsx
+++ b/public_html/excel_demo/packet-booking-demo.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Worksheet"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="70">
   <si>
     <t>awb_no</t>
   </si>
@@ -172,12 +172,6 @@
     <t>hello@yopmail.com</t>
   </si>
   <si>
-    <t>hfgdsfghsd</t>
-  </si>
-  <si>
-    <t>ICE 2</t>
-  </si>
-  <si>
     <t>DOX</t>
   </si>
   <si>
@@ -212,14 +206,31 @@
   </si>
   <si>
     <t>test 4</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>afghanistan</t>
+  </si>
+  <si>
+    <t>Shipping Charge</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Height</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,56 +279,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
+  <extLst xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
     <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
@@ -330,10 +337,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -371,71 +378,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -463,7 +470,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -486,11 +493,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -499,13 +506,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -515,7 +522,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -524,7 +531,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -533,7 +540,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -541,10 +548,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -609,68 +616,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:AW4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AE5" sqref="AE5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="41" max="41" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="42" max="42" style="13" width="22.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="43" max="43" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="44" max="44" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="45" max="45" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="46" max="46" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="47" max="47" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="48" max="48" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="49" max="49" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31" style="14" customWidth="1"/>
+    <col min="20" max="24" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="35" max="38" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="39" max="41" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="22.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="46" max="49" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:49" ht="19.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -761,17 +748,17 @@
       <c r="AD1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AE1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AH1" s="3" t="s">
-        <v>18</v>
+      <c r="AE1" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF1" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH1" s="14" t="s">
+        <v>69</v>
       </c>
       <c r="AI1" s="4" t="s">
         <v>21</v>
@@ -815,7 +802,7 @@
       <c r="AV1" s="4"/>
       <c r="AW1" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:49" ht="18.75" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -825,8 +812,8 @@
       <c r="C2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="7">
-        <v>1</v>
+      <c r="D2" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>37</v>
@@ -846,8 +833,8 @@
       <c r="J2" s="8">
         <v>393001</v>
       </c>
-      <c r="K2" s="8">
-        <v>1</v>
+      <c r="K2" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>41</v>
@@ -891,8 +878,8 @@
       <c r="Y2" s="8">
         <v>393002</v>
       </c>
-      <c r="Z2" s="8">
-        <v>2</v>
+      <c r="Z2" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="AA2" s="4" t="s">
         <v>49</v>
@@ -907,28 +894,28 @@
         <v>51</v>
       </c>
       <c r="AE2" s="8">
-        <v>124584545454</v>
-      </c>
-      <c r="AF2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF2" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AH2" s="8">
-        <v>152145214521452</v>
-      </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AK2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AL2" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="AK2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AL2" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="AM2" s="8">
         <v>12</v>
@@ -940,41 +927,41 @@
         <v>1500</v>
       </c>
       <c r="AP2" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AQ2" s="8">
         <v>3000</v>
       </c>
       <c r="AR2" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AS2" s="8">
         <v>45000</v>
       </c>
       <c r="AT2" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AU2" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AV2" s="4"/>
       <c r="AW2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:49" ht="18.75" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="7">
-        <v>2</v>
+      <c r="D3" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>37</v>
@@ -991,8 +978,8 @@
       <c r="J3" s="8">
         <v>393001</v>
       </c>
-      <c r="K3" s="8">
-        <v>1</v>
+      <c r="K3" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>41</v>
@@ -1036,8 +1023,8 @@
       <c r="Y3" s="8">
         <v>393002</v>
       </c>
-      <c r="Z3" s="8">
-        <v>2</v>
+      <c r="Z3" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="AA3" s="4" t="s">
         <v>49</v>
@@ -1052,28 +1039,28 @@
         <v>51</v>
       </c>
       <c r="AE3" s="8">
-        <v>124584545454</v>
-      </c>
-      <c r="AF3" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF3" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AG3" s="4" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AH3" s="8">
-        <v>152145214521452</v>
-      </c>
-      <c r="AI3" s="4" t="s">
+      <c r="AK3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AJ3" s="4" t="s">
+      <c r="AL3" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="AK3" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AL3" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="AM3" s="8">
         <v>12</v>
@@ -1085,29 +1072,29 @@
         <v>1500</v>
       </c>
       <c r="AP3" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AQ3" s="8">
         <v>3000</v>
       </c>
       <c r="AR3" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AS3" s="8">
         <v>45000</v>
       </c>
       <c r="AT3" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AU3" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AV3" s="4"/>
       <c r="AW3" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row r="4" spans="1:49" ht="19.5" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>35</v>
@@ -1115,14 +1102,14 @@
       <c r="C4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="2">
-        <v>3</v>
+      <c r="D4" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>37</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>38</v>
@@ -1136,8 +1123,8 @@
       <c r="J4" s="8">
         <v>393001</v>
       </c>
-      <c r="K4" s="8">
-        <v>1</v>
+      <c r="K4" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>41</v>
@@ -1181,8 +1168,8 @@
       <c r="Y4" s="8">
         <v>393002</v>
       </c>
-      <c r="Z4" s="8">
-        <v>2</v>
+      <c r="Z4" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="AA4" s="4" t="s">
         <v>49</v>
@@ -1197,28 +1184,28 @@
         <v>51</v>
       </c>
       <c r="AE4" s="8">
-        <v>124584545454</v>
-      </c>
-      <c r="AF4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="8">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AG4" s="4" t="s">
+      <c r="AJ4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AH4" s="8">
-        <v>152145214521452</v>
-      </c>
-      <c r="AI4" s="4" t="s">
+      <c r="AK4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AJ4" s="4" t="s">
+      <c r="AL4" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="AK4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AL4" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="AM4" s="8">
         <v>12</v>
@@ -1230,22 +1217,22 @@
         <v>1500</v>
       </c>
       <c r="AP4" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AQ4" s="8">
         <v>3000</v>
       </c>
       <c r="AR4" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AS4" s="8">
         <v>45000</v>
       </c>
       <c r="AT4" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AU4" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AV4" s="4"/>
       <c r="AW4" s="4"/>

</xml_diff>